<commit_message>
add forgot pass feature
</commit_message>
<xml_diff>
--- a/Bicycle-Rental/asset/user.xlsx
+++ b/Bicycle-Rental/asset/user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Temp\Bicycle-Rental\Bicycle-Rental\asset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\UIT\CS511\Bicycle-Rental\Bicycle-Rental\asset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078316F9-9C65-4AEF-824E-299A91849CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60772B9-213D-48E7-A361-3545FAD1DFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="0" windowWidth="9780" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,20 +403,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -454,7 +454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>

</xml_diff>